<commit_message>
change values according to new extraction parameters
</commit_message>
<xml_diff>
--- a/Radiomics_gliomas_article/data/D.xlsx
+++ b/Radiomics_gliomas_article/data/D.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tzaragori\Desktop\DOPA\Etudes\DOPA_Texture_Diag_init\Données\version_Article_propre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tzaragori\Desktop\DOPA\Code_git\Sklearn_NestedCV\master\Radiomics_gliomas_article\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF410A9-C45C-42A3-90A9-75D16BA901B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE44788-797A-4B30-A363-BAAA97578597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nestle" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -429,17 +429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C73"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -453,7 +450,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2">
@@ -464,7 +461,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
@@ -475,7 +472,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
@@ -486,7 +483,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
@@ -497,7 +494,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
@@ -508,7 +505,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
@@ -519,7 +516,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
@@ -530,18 +527,18 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>23.31666666666667</v>
       </c>
       <c r="C9">
-        <v>0.66541998959697568</v>
+        <v>0.56092948338929882</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
@@ -552,7 +549,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
@@ -563,7 +560,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
@@ -574,7 +571,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
@@ -585,7 +582,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14">
@@ -596,7 +593,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15">
@@ -607,7 +604,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16">
@@ -618,7 +615,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17">
@@ -629,7 +626,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18">
@@ -640,7 +637,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19">
@@ -651,7 +648,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20">
@@ -662,7 +659,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21">
@@ -673,7 +670,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22">
@@ -684,7 +681,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23">
@@ -695,7 +692,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24">
@@ -706,7 +703,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25">
@@ -717,7 +714,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26">
@@ -728,7 +725,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27">
@@ -739,7 +736,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28">
@@ -750,7 +747,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29">
@@ -761,7 +758,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30">
@@ -772,7 +769,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31">
@@ -783,7 +780,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32">
@@ -794,7 +791,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33">
@@ -805,7 +802,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34">
@@ -816,7 +813,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35">
@@ -827,7 +824,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36">
@@ -838,7 +835,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37">
@@ -849,7 +846,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38">
@@ -860,7 +857,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39">
@@ -871,7 +868,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40">
@@ -882,7 +879,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41">
@@ -893,7 +890,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42">
@@ -904,7 +901,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43">
@@ -915,7 +912,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44">
@@ -926,7 +923,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45">
@@ -937,7 +934,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46">
@@ -948,7 +945,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47">
@@ -959,7 +956,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48">
@@ -970,7 +967,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49">
@@ -981,7 +978,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50">
@@ -992,7 +989,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51">
@@ -1003,7 +1000,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52">
@@ -1014,7 +1011,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53">
@@ -1025,7 +1022,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54">
@@ -1036,7 +1033,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55">
@@ -1047,7 +1044,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56">
@@ -1058,7 +1055,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57">
@@ -1069,7 +1066,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58">
@@ -1080,7 +1077,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59">
@@ -1091,7 +1088,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60">
@@ -1102,7 +1099,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61">
@@ -1113,7 +1110,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62">
@@ -1124,7 +1121,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63">
@@ -1135,7 +1132,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64">
@@ -1146,7 +1143,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65">
@@ -1157,7 +1154,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66">
@@ -1168,7 +1165,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67">
@@ -1179,7 +1176,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68">
@@ -1190,7 +1187,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69">
@@ -1201,7 +1198,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70">
@@ -1212,7 +1209,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71">
@@ -1223,7 +1220,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72">
@@ -1234,7 +1231,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73">

</xml_diff>